<commit_message>
y-axis log(x+1) scale removed from biomass data. p-values rounded to 3 digits.
</commit_message>
<xml_diff>
--- a/Tables/PERMANOVA_bio_spInt_1.xlsx
+++ b/Tables/PERMANOVA_bio_spInt_1.xlsx
@@ -398,7 +398,7 @@
         <v>0.000661542462471505</v>
       </c>
       <c r="F2" t="n">
-        <v>0.7484</v>
+        <v>0.7554</v>
       </c>
     </row>
     <row r="3">
@@ -438,7 +438,7 @@
         <v>0.000982691586087769</v>
       </c>
       <c r="F4" t="n">
-        <v>0.7061</v>
+        <v>0.7074</v>
       </c>
     </row>
     <row r="5">
@@ -488,7 +488,7 @@
         <v>0.000128923623271053</v>
       </c>
       <c r="F7" t="n">
-        <v>0.8945</v>
+        <v>0.8939</v>
       </c>
     </row>
     <row r="8">
@@ -508,7 +508,7 @@
         <v>0.000849748466568212</v>
       </c>
       <c r="F8" t="n">
-        <v>0.7178</v>
+        <v>0.731</v>
       </c>
     </row>
     <row r="9">
@@ -528,7 +528,7 @@
         <v>0.00356599397678697</v>
       </c>
       <c r="F9" t="n">
-        <v>0.4702</v>
+        <v>0.4756</v>
       </c>
     </row>
     <row r="10">
@@ -578,7 +578,7 @@
         <v>0.000528796774183622</v>
       </c>
       <c r="F12" t="n">
-        <v>0.7743</v>
+        <v>0.7794</v>
       </c>
     </row>
     <row r="13">
@@ -598,7 +598,7 @@
         <v>0.000753262744555689</v>
       </c>
       <c r="F13" t="n">
-        <v>0.7436</v>
+        <v>0.7402</v>
       </c>
     </row>
     <row r="14">
@@ -618,7 +618,7 @@
         <v>0.0139371248267661</v>
       </c>
       <c r="F14" t="n">
-        <v>0.156</v>
+        <v>0.1598</v>
       </c>
     </row>
     <row r="15">
@@ -668,7 +668,7 @@
         <v>0.00000167917811929571</v>
       </c>
       <c r="F17" t="n">
-        <v>0.9891</v>
+        <v>0.9882</v>
       </c>
     </row>
     <row r="18">
@@ -688,7 +688,7 @@
         <v>0.010871573713867</v>
       </c>
       <c r="F18" t="n">
-        <v>0.2153</v>
+        <v>0.2101</v>
       </c>
     </row>
     <row r="19">
@@ -708,7 +708,7 @@
         <v>0.000651238487611556</v>
       </c>
       <c r="F19" t="n">
-        <v>0.7594</v>
+        <v>0.7577</v>
       </c>
     </row>
     <row r="20">
@@ -758,7 +758,7 @@
         <v>0.0197975649831835</v>
       </c>
       <c r="F22" t="n">
-        <v>0.0885</v>
+        <v>0.0813</v>
       </c>
     </row>
     <row r="23">
@@ -778,7 +778,7 @@
         <v>0.0265087988255299</v>
       </c>
       <c r="F23" t="n">
-        <v>0.0458</v>
+        <v>0.0469</v>
       </c>
     </row>
     <row r="24">
@@ -798,7 +798,7 @@
         <v>0.0145380870441804</v>
       </c>
       <c r="F24" t="n">
-        <v>0.139</v>
+        <v>0.1376</v>
       </c>
     </row>
     <row r="25">
@@ -848,7 +848,7 @@
         <v>0.000297998434895039</v>
       </c>
       <c r="F27" t="n">
-        <v>0.8402</v>
+        <v>0.8397</v>
       </c>
     </row>
     <row r="28">
@@ -868,7 +868,7 @@
         <v>0.000797703502359323</v>
       </c>
       <c r="F28" t="n">
-        <v>0.7345</v>
+        <v>0.7389</v>
       </c>
     </row>
     <row r="29">
@@ -888,7 +888,7 @@
         <v>0.00155715292871872</v>
       </c>
       <c r="F29" t="n">
-        <v>0.6313</v>
+        <v>0.6384</v>
       </c>
     </row>
     <row r="30">
@@ -938,7 +938,7 @@
         <v>0.000113899695877786</v>
       </c>
       <c r="F32" t="n">
-        <v>0.8937</v>
+        <v>0.8928</v>
       </c>
     </row>
     <row r="33">
@@ -958,7 +958,7 @@
         <v>0.0812962679545597</v>
       </c>
       <c r="F33" t="n">
-        <v>0.0005</v>
+        <v>0.0004</v>
       </c>
     </row>
     <row r="34">
@@ -978,7 +978,7 @@
         <v>0.0000676870230946712</v>
       </c>
       <c r="F34" t="n">
-        <v>0.9204</v>
+        <v>0.9191</v>
       </c>
     </row>
     <row r="35">
@@ -1028,7 +1028,7 @@
         <v>0.00135794570658376</v>
       </c>
       <c r="F37" t="n">
-        <v>0.696</v>
+        <v>0.6966</v>
       </c>
     </row>
     <row r="38">
@@ -1048,7 +1048,7 @@
         <v>0.0327056506250987</v>
       </c>
       <c r="F38" t="n">
-        <v>0.0496</v>
+        <v>0.0466</v>
       </c>
     </row>
     <row r="39">
@@ -1068,7 +1068,7 @@
         <v>0.00128647487992152</v>
       </c>
       <c r="F39" t="n">
-        <v>0.7337</v>
+        <v>0.7358</v>
       </c>
     </row>
     <row r="40">

</xml_diff>

<commit_message>
p-values rounded to three digits and for p < 0 on plots and permanova tables made anew.
</commit_message>
<xml_diff>
--- a/Tables/PERMANOVA_bio_spInt_1.xlsx
+++ b/Tables/PERMANOVA_bio_spInt_1.xlsx
@@ -398,7 +398,7 @@
         <v>0.000661542462471505</v>
       </c>
       <c r="F2" t="n">
-        <v>0.7554</v>
+        <v>0.7564</v>
       </c>
     </row>
     <row r="3">
@@ -418,7 +418,7 @@
         <v>0.0624915990055264</v>
       </c>
       <c r="F3" t="n">
-        <v>0.0018</v>
+        <v>0.0011</v>
       </c>
     </row>
     <row r="4">
@@ -438,7 +438,7 @@
         <v>0.000982691586087769</v>
       </c>
       <c r="F4" t="n">
-        <v>0.7074</v>
+        <v>0.6979</v>
       </c>
     </row>
     <row r="5">
@@ -488,7 +488,7 @@
         <v>0.000128923623271053</v>
       </c>
       <c r="F7" t="n">
-        <v>0.8939</v>
+        <v>0.8914</v>
       </c>
     </row>
     <row r="8">
@@ -508,7 +508,7 @@
         <v>0.000849748466568212</v>
       </c>
       <c r="F8" t="n">
-        <v>0.731</v>
+        <v>0.7299</v>
       </c>
     </row>
     <row r="9">
@@ -528,7 +528,7 @@
         <v>0.00356599397678697</v>
       </c>
       <c r="F9" t="n">
-        <v>0.4756</v>
+        <v>0.4701</v>
       </c>
     </row>
     <row r="10">
@@ -578,7 +578,7 @@
         <v>0.000528796774183622</v>
       </c>
       <c r="F12" t="n">
-        <v>0.7794</v>
+        <v>0.7775</v>
       </c>
     </row>
     <row r="13">
@@ -598,7 +598,7 @@
         <v>0.000753262744555689</v>
       </c>
       <c r="F13" t="n">
-        <v>0.7402</v>
+        <v>0.7392</v>
       </c>
     </row>
     <row r="14">
@@ -618,7 +618,7 @@
         <v>0.0139371248267661</v>
       </c>
       <c r="F14" t="n">
-        <v>0.1598</v>
+        <v>0.1559</v>
       </c>
     </row>
     <row r="15">
@@ -668,7 +668,7 @@
         <v>0.00000167917811929571</v>
       </c>
       <c r="F17" t="n">
-        <v>0.9882</v>
+        <v>0.9872</v>
       </c>
     </row>
     <row r="18">
@@ -688,7 +688,7 @@
         <v>0.010871573713867</v>
       </c>
       <c r="F18" t="n">
-        <v>0.2101</v>
+        <v>0.2022</v>
       </c>
     </row>
     <row r="19">
@@ -708,7 +708,7 @@
         <v>0.000651238487611556</v>
       </c>
       <c r="F19" t="n">
-        <v>0.7577</v>
+        <v>0.7552</v>
       </c>
     </row>
     <row r="20">
@@ -758,7 +758,7 @@
         <v>0.0197975649831835</v>
       </c>
       <c r="F22" t="n">
-        <v>0.0813</v>
+        <v>0.0859</v>
       </c>
     </row>
     <row r="23">
@@ -778,7 +778,7 @@
         <v>0.0265087988255299</v>
       </c>
       <c r="F23" t="n">
-        <v>0.0469</v>
+        <v>0.0453</v>
       </c>
     </row>
     <row r="24">
@@ -798,7 +798,7 @@
         <v>0.0145380870441804</v>
       </c>
       <c r="F24" t="n">
-        <v>0.1376</v>
+        <v>0.1371</v>
       </c>
     </row>
     <row r="25">
@@ -848,7 +848,7 @@
         <v>0.000297998434895039</v>
       </c>
       <c r="F27" t="n">
-        <v>0.8397</v>
+        <v>0.8272</v>
       </c>
     </row>
     <row r="28">
@@ -868,7 +868,7 @@
         <v>0.000797703502359323</v>
       </c>
       <c r="F28" t="n">
-        <v>0.7389</v>
+        <v>0.7351</v>
       </c>
     </row>
     <row r="29">
@@ -888,7 +888,7 @@
         <v>0.00155715292871872</v>
       </c>
       <c r="F29" t="n">
-        <v>0.6384</v>
+        <v>0.6332</v>
       </c>
     </row>
     <row r="30">
@@ -938,7 +938,7 @@
         <v>0.000113899695877786</v>
       </c>
       <c r="F32" t="n">
-        <v>0.8928</v>
+        <v>0.8977</v>
       </c>
     </row>
     <row r="33">
@@ -958,7 +958,7 @@
         <v>0.0812962679545597</v>
       </c>
       <c r="F33" t="n">
-        <v>0.0004</v>
+        <v>0.0006</v>
       </c>
     </row>
     <row r="34">
@@ -978,7 +978,7 @@
         <v>0.0000676870230946712</v>
       </c>
       <c r="F34" t="n">
-        <v>0.9191</v>
+        <v>0.9203</v>
       </c>
     </row>
     <row r="35">
@@ -1028,7 +1028,7 @@
         <v>0.00135794570658376</v>
       </c>
       <c r="F37" t="n">
-        <v>0.6966</v>
+        <v>0.6905</v>
       </c>
     </row>
     <row r="38">
@@ -1048,7 +1048,7 @@
         <v>0.0327056506250987</v>
       </c>
       <c r="F38" t="n">
-        <v>0.0466</v>
+        <v>0.0524</v>
       </c>
     </row>
     <row r="39">
@@ -1068,7 +1068,7 @@
         <v>0.00128647487992152</v>
       </c>
       <c r="F39" t="n">
-        <v>0.7358</v>
+        <v>0.7377</v>
       </c>
     </row>
     <row r="40">

</xml_diff>